<commit_message>
basic file uploads, some work towards #14
</commit_message>
<xml_diff>
--- a/documentation/Example files/survey_signal.xlsx
+++ b/documentation/Example files/survey_signal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>cool</t>
   </si>
@@ -125,6 +125,36 @@
   </si>
   <si>
     <t>RT</t>
+  </si>
+  <si>
+    <t>geopoint</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Record your location</t>
+  </si>
+  <si>
+    <t>rating_button</t>
+  </si>
+  <si>
+    <t>agreement</t>
+  </si>
+  <si>
+    <t>Do you agree that SurveySignal is cool &amp; hip?</t>
+  </si>
+  <si>
+    <t>choice1</t>
+  </si>
+  <si>
+    <t>choice2</t>
+  </si>
+  <si>
+    <t>&lt;i class="fa fa-smile-o fa-2x"&gt;&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>&lt;i class="fa fa-meh-o fa-2x"&gt;&lt;/i&gt;</t>
   </si>
 </sst>
 </file>
@@ -566,11 +596,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -581,7 +611,7 @@
     <col min="4" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="18">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="18">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -591,8 +621,14 @@
       <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
@@ -600,7 +636,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -608,7 +644,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -616,7 +652,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -624,7 +660,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
@@ -632,7 +668,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:5">
       <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
@@ -640,7 +676,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:5">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
@@ -648,7 +684,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:5">
       <c r="A9" s="5" t="s">
         <v>29</v>
       </c>
@@ -656,7 +692,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:5">
       <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
@@ -664,12 +700,40 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:5">
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45">
+      <c r="A13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>